<commit_message>
Added RTM and all minutes of meeting
</commit_message>
<xml_diff>
--- a/RTM/RTM_KS.1.xlsx
+++ b/RTM/RTM_KS.1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25712"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="84" documentId="11_37263EFE396C61F98BE08B4A8D3C3C264B0043C9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3589F65C-AD28-4268-8CD5-4FF61DC6E20E}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="11_37263EFE396C61F98BE08B4A8D3C3C264B0043C9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7520676-A1BD-46C9-B27D-DEB60EDC6C10}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Req</t>
   </si>
@@ -51,7 +51,7 @@
     <t>3.1.1</t>
   </si>
   <si>
-    <t>file_parsing()</t>
+    <t>file_validation()</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -66,92 +66,92 @@
     <t>3.1.2</t>
   </si>
   <si>
-    <t>file_validation()</t>
+    <t>file_validation(), extract_project_details()</t>
+  </si>
+  <si>
+    <t>IT_CASE2</t>
+  </si>
+  <si>
+    <t>KS_03</t>
+  </si>
+  <si>
+    <t>3.1.3</t>
   </si>
   <si>
     <t>Unit Test Case1_6</t>
   </si>
   <si>
-    <t>IT_CASE2</t>
-  </si>
-  <si>
-    <t>KS_03</t>
-  </si>
-  <si>
-    <t>3.1.3</t>
+    <t>IT_CASE3</t>
+  </si>
+  <si>
+    <t>KS_04</t>
+  </si>
+  <si>
+    <t>3.1.4</t>
+  </si>
+  <si>
+    <t>extract_project_details()</t>
+  </si>
+  <si>
+    <t>IT_CASE4</t>
+  </si>
+  <si>
+    <t>KS_05</t>
+  </si>
+  <si>
+    <t>3.1.5</t>
+  </si>
+  <si>
+    <t>keyword_search()</t>
+  </si>
+  <si>
+    <t>IT_CASE1, IT_CASE2</t>
+  </si>
+  <si>
+    <t>KS_06</t>
+  </si>
+  <si>
+    <t>3.1.6</t>
+  </si>
+  <si>
+    <t>display_result()</t>
+  </si>
+  <si>
+    <t>IT_CASE6</t>
+  </si>
+  <si>
+    <t>KS_07</t>
+  </si>
+  <si>
+    <t>3.1.7</t>
+  </si>
+  <si>
+    <t>store_result()</t>
+  </si>
+  <si>
+    <t>Unit Test Case7_12</t>
+  </si>
+  <si>
+    <t>IT_CASE7</t>
+  </si>
+  <si>
+    <t>KS_08</t>
+  </si>
+  <si>
+    <t>3.1.8</t>
   </si>
   <si>
     <t>display_invalid()</t>
   </si>
   <si>
-    <t>IT_CASE3</t>
-  </si>
-  <si>
-    <t>KS_04</t>
-  </si>
-  <si>
-    <t>3.1.4</t>
-  </si>
-  <si>
-    <t>extract_project_details()</t>
-  </si>
-  <si>
-    <t>IT_CASE4</t>
-  </si>
-  <si>
-    <t>KS_05</t>
-  </si>
-  <si>
-    <t>3.1.5</t>
-  </si>
-  <si>
-    <t>keyword_search()</t>
-  </si>
-  <si>
     <t>IT_CASE5</t>
-  </si>
-  <si>
-    <t>KS_06</t>
-  </si>
-  <si>
-    <t>3.1.6</t>
-  </si>
-  <si>
-    <t>display_result()</t>
-  </si>
-  <si>
-    <t>IT_CASE6</t>
-  </si>
-  <si>
-    <t>KS_07</t>
-  </si>
-  <si>
-    <t>3.1.7</t>
-  </si>
-  <si>
-    <t>store_result()</t>
-  </si>
-  <si>
-    <t>IT_CASE7</t>
-  </si>
-  <si>
-    <t>KS_08</t>
-  </si>
-  <si>
-    <t>3.1.8</t>
-  </si>
-  <si>
-    <t>valid_result()</t>
-  </si>
-  <si>
-    <t>Unit Test Case7_12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,6 +183,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -246,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -265,6 +272,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,7 +491,7 @@
   <dimension ref="A1:H997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -530,7 +538,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" ht="30.75">
       <c r="A3" s="8" t="s">
         <v>10</v>
       </c>
@@ -540,84 +548,86 @@
       <c r="C3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="E4" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>21</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="C6" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="C7" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="C8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="6"/>
       <c r="E8" s="3" t="s">
         <v>34</v>
       </c>
@@ -632,10 +642,9 @@
       <c r="C9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="3"/>
@@ -1658,15 +1667,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="023f1dae-eefa-4464-9427-685eeabbe412">
@@ -1674,6 +1674,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1849,11 +1858,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{603FF8AA-530F-4BC8-94E9-41C5994D370F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03B51193-3DFC-4939-A5DB-8BC564912C4B}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03B51193-3DFC-4939-A5DB-8BC564912C4B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{603FF8AA-530F-4BC8-94E9-41C5994D370F}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>